<commit_message>
fixed nums row, add 2 row down and up over R
</commit_message>
<xml_diff>
--- a/DLVAA4033026 (1).xlsx
+++ b/DLVAA4033026 (1).xlsx
@@ -670,11 +670,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="176" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="180" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -704,6 +704,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -711,7 +718,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -720,13 +727,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -741,10 +741,41 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -771,17 +802,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -795,29 +826,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -825,7 +833,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -835,13 +842,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -856,13 +856,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -874,7 +868,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,7 +898,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,19 +910,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -922,7 +928,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -940,7 +946,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -952,73 +994,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,7 +1018,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1080,6 +1080,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1091,6 +1100,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1121,24 +1139,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1165,154 +1165,154 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1334,10 +1334,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1346,7 +1346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1358,7 +1358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1707,13 +1707,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr filterMode="1" codeName="Лист1">
+  <sheetPr codeName="Лист1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="$A52:$XFD127"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1786,7 +1786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" ht="51" hidden="1" spans="1:15">
+    <row r="3" ht="51" spans="1:15">
       <c r="A3" s="5">
         <f t="shared" ref="A3:A66" si="0">IF(A2="№ п/п",1,A2+1)</f>
         <v>1</v>
@@ -1835,7 +1835,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" ht="38.25" hidden="1" spans="1:15">
+    <row r="4" ht="38.25" spans="1:15">
       <c r="A4" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1850,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="6">
-        <v>825</v>
+        <v>999</v>
       </c>
       <c r="F4" s="8">
         <v>2084642</v>
@@ -1884,7 +1884,7 @@
         <v>8251006179</v>
       </c>
     </row>
-    <row r="5" ht="38.25" hidden="1" spans="1:15">
+    <row r="5" ht="38.25" spans="1:15">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1933,7 +1933,7 @@
         <v>8251006338</v>
       </c>
     </row>
-    <row r="6" ht="38.25" hidden="1" spans="1:15">
+    <row r="6" ht="38.25" spans="1:15">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1982,7 +1982,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" ht="38.25" hidden="1" spans="1:15">
+    <row r="7" ht="38.25" spans="1:15">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2031,7 +2031,7 @@
         <v>8251006402</v>
       </c>
     </row>
-    <row r="8" ht="38.25" hidden="1" spans="1:15">
+    <row r="8" ht="38.25" spans="1:15">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2080,7 +2080,7 @@
         <v>8251006282</v>
       </c>
     </row>
-    <row r="9" ht="38.25" hidden="1" spans="1:15">
+    <row r="9" ht="38.25" spans="1:15">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2129,7 +2129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" ht="38.25" hidden="1" spans="1:15">
+    <row r="10" ht="38.25" spans="1:15">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2178,7 +2178,7 @@
         <v>8251006466</v>
       </c>
     </row>
-    <row r="11" ht="38.25" hidden="1" spans="1:15">
+    <row r="11" ht="38.25" spans="1:15">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2227,7 +2227,7 @@
         <v>8251006351</v>
       </c>
     </row>
-    <row r="12" ht="38.25" hidden="1" spans="1:15">
+    <row r="12" ht="38.25" spans="1:15">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2276,7 +2276,7 @@
         <v>8251006471</v>
       </c>
     </row>
-    <row r="13" ht="38.25" hidden="1" spans="1:15">
+    <row r="13" ht="38.25" spans="1:15">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2325,7 +2325,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" ht="63.75" hidden="1" spans="1:15">
+    <row r="14" ht="63.75" spans="1:15">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2374,7 +2374,7 @@
         <v>8251006490</v>
       </c>
     </row>
-    <row r="15" ht="51" hidden="1" spans="1:15">
+    <row r="15" ht="51" spans="1:15">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2423,7 +2423,7 @@
         <v>8251006534</v>
       </c>
     </row>
-    <row r="16" ht="38.25" hidden="1" spans="1:15">
+    <row r="16" ht="38.25" spans="1:15">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2472,7 +2472,7 @@
         <v>8251006484</v>
       </c>
     </row>
-    <row r="17" ht="38.25" hidden="1" spans="1:15">
+    <row r="17" ht="38.25" spans="1:15">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2521,7 +2521,7 @@
         <v>8251006484</v>
       </c>
     </row>
-    <row r="18" ht="38.25" hidden="1" spans="1:15">
+    <row r="18" ht="38.25" spans="1:15">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2570,7 +2570,7 @@
         <v>8251006415</v>
       </c>
     </row>
-    <row r="19" ht="38.25" hidden="1" spans="1:15">
+    <row r="19" ht="38.25" spans="1:15">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2619,7 +2619,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" ht="38.25" hidden="1" spans="1:15">
+    <row r="20" ht="38.25" spans="1:15">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2668,7 +2668,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" ht="38.25" hidden="1" spans="1:15">
+    <row r="21" ht="38.25" spans="1:15">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2717,7 +2717,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" ht="38.25" hidden="1" spans="1:15">
+    <row r="22" ht="38.25" spans="1:15">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2766,7 +2766,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" ht="38.25" hidden="1" spans="1:15">
+    <row r="23" ht="38.25" spans="1:15">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2815,7 +2815,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" ht="38.25" hidden="1" spans="1:15">
+    <row r="24" ht="38.25" spans="1:15">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2864,7 +2864,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" ht="38.25" hidden="1" spans="1:15">
+    <row r="25" ht="38.25" spans="1:15">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2913,7 +2913,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" ht="38.25" hidden="1" spans="1:15">
+    <row r="26" ht="38.25" spans="1:15">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2962,7 +2962,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" ht="38.25" hidden="1" spans="1:15">
+    <row r="27" ht="38.25" spans="1:15">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3011,7 +3011,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" ht="38.25" hidden="1" spans="1:15">
+    <row r="28" ht="38.25" spans="1:15">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3060,7 +3060,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" ht="38.25" hidden="1" spans="1:15">
+    <row r="29" ht="38.25" spans="1:15">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3109,7 +3109,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" ht="38.25" hidden="1" spans="1:15">
+    <row r="30" ht="38.25" spans="1:15">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3158,7 +3158,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" ht="38.25" hidden="1" spans="1:15">
+    <row r="31" ht="38.25" spans="1:15">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3207,7 +3207,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" ht="38.25" hidden="1" spans="1:15">
+    <row r="32" ht="38.25" spans="1:15">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3256,7 +3256,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" ht="38.25" hidden="1" spans="1:15">
+    <row r="33" ht="38.25" spans="1:15">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3305,7 +3305,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" ht="38.25" hidden="1" spans="1:15">
+    <row r="34" ht="38.25" spans="1:15">
       <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3354,7 +3354,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" ht="38.25" hidden="1" spans="1:15">
+    <row r="35" ht="38.25" spans="1:15">
       <c r="A35" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3403,7 +3403,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" ht="38.25" hidden="1" spans="1:15">
+    <row r="36" ht="38.25" spans="1:15">
       <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3452,7 +3452,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" ht="38.25" hidden="1" spans="1:15">
+    <row r="37" ht="38.25" spans="1:15">
       <c r="A37" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3501,7 +3501,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" ht="38.25" hidden="1" spans="1:15">
+    <row r="38" ht="38.25" spans="1:15">
       <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3550,7 +3550,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" ht="38.25" hidden="1" spans="1:15">
+    <row r="39" ht="38.25" spans="1:15">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3599,7 +3599,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" ht="38.25" hidden="1" spans="1:15">
+    <row r="40" ht="38.25" spans="1:15">
       <c r="A40" s="5">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3648,7 +3648,7 @@
         <v>8251006619</v>
       </c>
     </row>
-    <row r="41" ht="38.25" hidden="1" spans="1:15">
+    <row r="41" ht="38.25" spans="1:15">
       <c r="A41" s="5">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3697,7 +3697,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" ht="38.25" hidden="1" spans="1:15">
+    <row r="42" ht="38.25" spans="1:15">
       <c r="A42" s="5">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3746,7 +3746,7 @@
         <v>8251006486</v>
       </c>
     </row>
-    <row r="43" ht="38.25" hidden="1" spans="1:15">
+    <row r="43" ht="38.25" spans="1:15">
       <c r="A43" s="5">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3795,7 +3795,7 @@
         <v>8251006543</v>
       </c>
     </row>
-    <row r="44" ht="76.5" hidden="1" spans="1:15">
+    <row r="44" ht="76.5" spans="1:15">
       <c r="A44" s="5">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3844,7 +3844,7 @@
         <v>8251006559</v>
       </c>
     </row>
-    <row r="45" ht="51" hidden="1" spans="1:15">
+    <row r="45" ht="51" spans="1:15">
       <c r="A45" s="5">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3893,7 +3893,7 @@
         <v>8251006363</v>
       </c>
     </row>
-    <row r="46" ht="51" hidden="1" spans="1:15">
+    <row r="46" ht="51" spans="1:15">
       <c r="A46" s="5">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3942,7 +3942,7 @@
         <v>8251006363</v>
       </c>
     </row>
-    <row r="47" ht="51" hidden="1" spans="1:15">
+    <row r="47" ht="51" spans="1:15">
       <c r="A47" s="5">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3991,7 +3991,7 @@
         <v>8251006363</v>
       </c>
     </row>
-    <row r="48" ht="51" hidden="1" spans="1:15">
+    <row r="48" ht="51" spans="1:15">
       <c r="A48" s="5">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -4040,7 +4040,7 @@
         <v>8251006363</v>
       </c>
     </row>
-    <row r="49" ht="51" hidden="1" spans="1:15">
+    <row r="49" ht="51" spans="1:15">
       <c r="A49" s="5">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4089,7 +4089,7 @@
         <v>8251006363</v>
       </c>
     </row>
-    <row r="50" ht="38.25" hidden="1" spans="1:15">
+    <row r="50" ht="38.25" spans="1:15">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4138,7 +4138,7 @@
         <v>8251006598</v>
       </c>
     </row>
-    <row r="51" ht="51" hidden="1" spans="1:15">
+    <row r="51" ht="51" spans="1:15">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4187,7 +4187,7 @@
         <v>8251006558</v>
       </c>
     </row>
-    <row r="52" ht="51" hidden="1" spans="1:15">
+    <row r="52" ht="51" spans="1:15">
       <c r="A52" s="5" t="e">
         <f>IF(#REF!="№ п/п",1,#REF!+1)</f>
         <v>#REF!</v>
@@ -4236,9 +4236,9 @@
         <v>8251006558</v>
       </c>
     </row>
-    <row r="53" ht="51" hidden="1" spans="1:15">
+    <row r="53" ht="51" spans="1:15">
       <c r="A53" s="5" t="e">
-        <f>IF(A52="№ п/п",1,A52+1)</f>
+        <f t="shared" ref="A53:A65" si="3">IF(A52="№ п/п",1,A52+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -4285,9 +4285,9 @@
         <v>8251006558</v>
       </c>
     </row>
-    <row r="54" ht="51" hidden="1" spans="1:15">
+    <row r="54" ht="51" spans="1:15">
       <c r="A54" s="5" t="e">
-        <f>IF(A53="№ п/п",1,A53+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B54" s="6" t="s">
@@ -4334,9 +4334,9 @@
         <v>8251006558</v>
       </c>
     </row>
-    <row r="55" ht="51" hidden="1" spans="1:15">
+    <row r="55" ht="51" spans="1:15">
       <c r="A55" s="5" t="e">
-        <f>IF(A54="№ п/п",1,A54+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B55" s="6" t="s">
@@ -4383,9 +4383,9 @@
         <v>8251006558</v>
       </c>
     </row>
-    <row r="56" ht="51" hidden="1" spans="1:15">
+    <row r="56" ht="51" spans="1:15">
       <c r="A56" s="5" t="e">
-        <f>IF(A55="№ п/п",1,A55+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -4432,9 +4432,9 @@
         <v>8251006558</v>
       </c>
     </row>
-    <row r="57" ht="38.25" hidden="1" spans="1:15">
+    <row r="57" ht="38.25" spans="1:15">
       <c r="A57" s="5" t="e">
-        <f>IF(A56="№ п/п",1,A56+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -4481,9 +4481,9 @@
         <v>8251006514</v>
       </c>
     </row>
-    <row r="58" ht="38.25" hidden="1" spans="1:15">
+    <row r="58" ht="38.25" spans="1:15">
       <c r="A58" s="5" t="e">
-        <f>IF(A57="№ п/п",1,A57+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B58" s="6" t="s">
@@ -4530,9 +4530,9 @@
         <v>8251006514</v>
       </c>
     </row>
-    <row r="59" ht="38.25" hidden="1" spans="1:15">
+    <row r="59" ht="38.25" spans="1:15">
       <c r="A59" s="5" t="e">
-        <f>IF(A58="№ п/п",1,A58+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B59" s="6" t="s">
@@ -4579,9 +4579,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" ht="38.25" hidden="1" spans="1:15">
+    <row r="60" ht="38.25" spans="1:15">
       <c r="A60" s="5" t="e">
-        <f>IF(A59="№ п/п",1,A59+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B60" s="6" t="s">
@@ -4628,9 +4628,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" ht="38.25" hidden="1" spans="1:15">
+    <row r="61" ht="38.25" spans="1:15">
       <c r="A61" s="5" t="e">
-        <f>IF(A60="№ п/п",1,A60+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B61" s="6" t="s">
@@ -4677,9 +4677,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" ht="38.25" hidden="1" spans="1:15">
+    <row r="62" ht="38.25" spans="1:15">
       <c r="A62" s="5" t="e">
-        <f>IF(A61="№ п/п",1,A61+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -4726,9 +4726,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" ht="38.25" hidden="1" spans="1:15">
+    <row r="63" ht="38.25" spans="1:15">
       <c r="A63" s="5" t="e">
-        <f>IF(A62="№ п/п",1,A62+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B63" s="6" t="s">
@@ -4775,9 +4775,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="64" ht="38.25" hidden="1" spans="1:15">
+    <row r="64" ht="38.25" spans="1:15">
       <c r="A64" s="5" t="e">
-        <f>IF(A63="№ п/п",1,A63+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B64" s="6" t="s">
@@ -4824,9 +4824,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" ht="38.25" hidden="1" spans="1:15">
+    <row r="65" ht="38.25" spans="1:15">
       <c r="A65" s="5" t="e">
-        <f>IF(A64="№ п/п",1,A64+1)</f>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="B65" s="6" t="s">
@@ -4873,9 +4873,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" ht="38.25" hidden="1" spans="1:15">
+    <row r="66" ht="38.25" spans="1:15">
       <c r="A66" s="5" t="e">
-        <f t="shared" ref="A66:A97" si="3">IF(A65="№ п/п",1,A65+1)</f>
+        <f t="shared" ref="A66:A97" si="4">IF(A65="№ п/п",1,A65+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B66" s="6" t="s">
@@ -4922,9 +4922,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" ht="51" hidden="1" spans="1:15">
+    <row r="67" ht="51" spans="1:15">
       <c r="A67" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B67" s="6" t="s">
@@ -4971,9 +4971,9 @@
         <v>8251006336</v>
       </c>
     </row>
-    <row r="68" ht="51" hidden="1" spans="1:15">
+    <row r="68" ht="51" spans="1:15">
       <c r="A68" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B68" s="6" t="s">
@@ -5020,9 +5020,9 @@
         <v>8251006336</v>
       </c>
     </row>
-    <row r="69" ht="51" hidden="1" spans="1:15">
+    <row r="69" ht="51" spans="1:15">
       <c r="A69" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B69" s="6" t="s">
@@ -5069,9 +5069,9 @@
         <v>8251006336</v>
       </c>
     </row>
-    <row r="70" ht="51" hidden="1" spans="1:15">
+    <row r="70" ht="51" spans="1:15">
       <c r="A70" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B70" s="6" t="s">
@@ -5118,9 +5118,9 @@
         <v>8251006387</v>
       </c>
     </row>
-    <row r="71" ht="38.25" hidden="1" spans="1:15">
+    <row r="71" ht="38.25" spans="1:15">
       <c r="A71" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B71" s="6" t="s">
@@ -5167,9 +5167,9 @@
         <v>8251006487</v>
       </c>
     </row>
-    <row r="72" ht="38.25" hidden="1" spans="1:15">
+    <row r="72" ht="38.25" spans="1:15">
       <c r="A72" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B72" s="6" t="s">
@@ -5216,9 +5216,9 @@
         <v>8251006666</v>
       </c>
     </row>
-    <row r="73" ht="51" hidden="1" spans="1:15">
+    <row r="73" ht="51" spans="1:15">
       <c r="A73" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B73" s="6" t="s">
@@ -5265,9 +5265,9 @@
         <v>8251006433</v>
       </c>
     </row>
-    <row r="74" ht="51" hidden="1" spans="1:15">
+    <row r="74" ht="51" spans="1:15">
       <c r="A74" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B74" s="6" t="s">
@@ -5314,9 +5314,9 @@
         <v>8251006433</v>
       </c>
     </row>
-    <row r="75" ht="51" hidden="1" spans="1:15">
+    <row r="75" ht="51" spans="1:15">
       <c r="A75" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -5363,9 +5363,9 @@
         <v>8251006433</v>
       </c>
     </row>
-    <row r="76" ht="51" hidden="1" spans="1:15">
+    <row r="76" ht="51" spans="1:15">
       <c r="A76" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B76" s="6" t="s">
@@ -5412,9 +5412,9 @@
         <v>8251006433</v>
       </c>
     </row>
-    <row r="77" ht="51" hidden="1" spans="1:15">
+    <row r="77" ht="51" spans="1:15">
       <c r="A77" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B77" s="6" t="s">
@@ -5461,9 +5461,9 @@
         <v>8251006433</v>
       </c>
     </row>
-    <row r="78" ht="51" hidden="1" spans="1:15">
+    <row r="78" ht="51" spans="1:15">
       <c r="A78" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B78" s="6" t="s">
@@ -5510,9 +5510,9 @@
         <v>8251006433</v>
       </c>
     </row>
-    <row r="79" ht="51" hidden="1" spans="1:15">
+    <row r="79" ht="51" spans="1:15">
       <c r="A79" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B79" s="6" t="s">
@@ -5559,9 +5559,9 @@
         <v>8251006433</v>
       </c>
     </row>
-    <row r="80" ht="38.25" hidden="1" spans="1:15">
+    <row r="80" ht="38.25" spans="1:15">
       <c r="A80" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B80" s="6" t="s">
@@ -5608,9 +5608,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="81" ht="38.25" hidden="1" spans="1:15">
+    <row r="81" ht="38.25" spans="1:15">
       <c r="A81" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B81" s="6" t="s">
@@ -5657,9 +5657,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" ht="38.25" hidden="1" spans="1:15">
+    <row r="82" ht="38.25" spans="1:15">
       <c r="A82" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B82" s="6" t="s">
@@ -5706,9 +5706,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" ht="38.25" hidden="1" spans="1:15">
+    <row r="83" ht="38.25" spans="1:15">
       <c r="A83" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B83" s="6" t="s">
@@ -5748,16 +5748,16 @@
         <v>51</v>
       </c>
       <c r="N83" s="13" t="str">
-        <f t="shared" ref="N83:N89" si="4">"C1350693"</f>
+        <f t="shared" ref="N83:N89" si="5">"C1350693"</f>
         <v>C1350693</v>
       </c>
       <c r="O83" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="84" ht="38.25" hidden="1" spans="1:15">
+    <row r="84" ht="38.25" spans="1:15">
       <c r="A84" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B84" s="6" t="s">
@@ -5797,16 +5797,16 @@
         <v>51</v>
       </c>
       <c r="N84" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C1350693</v>
       </c>
       <c r="O84" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="85" ht="38.25" hidden="1" spans="1:15">
+    <row r="85" ht="38.25" spans="1:15">
       <c r="A85" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B85" s="6" t="s">
@@ -5846,16 +5846,16 @@
         <v>51</v>
       </c>
       <c r="N85" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C1350693</v>
       </c>
       <c r="O85" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="86" ht="38.25" hidden="1" spans="1:15">
+    <row r="86" ht="38.25" spans="1:15">
       <c r="A86" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B86" s="6" t="s">
@@ -5895,16 +5895,16 @@
         <v>51</v>
       </c>
       <c r="N86" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C1350693</v>
       </c>
       <c r="O86" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="87" ht="38.25" hidden="1" spans="1:15">
+    <row r="87" ht="38.25" spans="1:15">
       <c r="A87" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B87" s="6" t="s">
@@ -5944,16 +5944,16 @@
         <v>51</v>
       </c>
       <c r="N87" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C1350693</v>
       </c>
       <c r="O87" s="14">
         <v>8251006550</v>
       </c>
     </row>
-    <row r="88" ht="38.25" hidden="1" spans="1:15">
+    <row r="88" ht="38.25" spans="1:15">
       <c r="A88" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B88" s="6" t="s">
@@ -5993,16 +5993,16 @@
         <v>51</v>
       </c>
       <c r="N88" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C1350693</v>
       </c>
       <c r="O88" s="14">
         <v>8251006550</v>
       </c>
     </row>
-    <row r="89" ht="38.25" hidden="1" spans="1:15">
+    <row r="89" ht="38.25" spans="1:15">
       <c r="A89" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B89" s="6" t="s">
@@ -6042,16 +6042,16 @@
         <v>51</v>
       </c>
       <c r="N89" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C1350693</v>
       </c>
       <c r="O89" s="14">
         <v>8251006550</v>
       </c>
     </row>
-    <row r="90" ht="38.25" hidden="1" spans="1:15">
+    <row r="90" ht="38.25" spans="1:15">
       <c r="A90" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B90" s="6" t="s">
@@ -6098,9 +6098,9 @@
         <v>8251006602</v>
       </c>
     </row>
-    <row r="91" ht="38.25" hidden="1" spans="1:15">
+    <row r="91" ht="38.25" spans="1:15">
       <c r="A91" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B91" s="6" t="s">
@@ -6147,9 +6147,9 @@
         <v>8251006602</v>
       </c>
     </row>
-    <row r="92" ht="38.25" hidden="1" spans="1:15">
+    <row r="92" ht="38.25" spans="1:15">
       <c r="A92" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B92" s="6" t="s">
@@ -6196,9 +6196,9 @@
         <v>8251006602</v>
       </c>
     </row>
-    <row r="93" ht="38.25" hidden="1" spans="1:15">
+    <row r="93" ht="38.25" spans="1:15">
       <c r="A93" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B93" s="6" t="s">
@@ -6245,9 +6245,9 @@
         <v>8251006653</v>
       </c>
     </row>
-    <row r="94" ht="38.25" hidden="1" spans="1:15">
+    <row r="94" ht="38.25" spans="1:15">
       <c r="A94" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B94" s="6" t="s">
@@ -6294,9 +6294,9 @@
         <v>8251006491</v>
       </c>
     </row>
-    <row r="95" ht="114.75" hidden="1" spans="1:15">
+    <row r="95" ht="114.75" spans="1:15">
       <c r="A95" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B95" s="6" t="s">
@@ -6343,9 +6343,9 @@
         <v>162</v>
       </c>
     </row>
-    <row r="96" ht="114.75" hidden="1" spans="1:15">
+    <row r="96" ht="114.75" spans="1:15">
       <c r="A96" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B96" s="6" t="s">
@@ -6392,9 +6392,9 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" ht="38.25" hidden="1" spans="1:15">
+    <row r="97" ht="38.25" spans="1:15">
       <c r="A97" s="5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="B97" s="6" t="s">
@@ -6441,7 +6441,7 @@
         <v>8251006621</v>
       </c>
     </row>
-    <row r="98" ht="38.25" hidden="1" spans="1:15">
+    <row r="98" ht="38.25" spans="1:15">
       <c r="A98" s="5" t="e">
         <f>IF(#REF!="№ п/п",1,#REF!+1)</f>
         <v>#REF!</v>
@@ -6490,9 +6490,9 @@
         <v>8251006552</v>
       </c>
     </row>
-    <row r="99" ht="51" hidden="1" spans="1:15">
+    <row r="99" ht="51" spans="1:15">
       <c r="A99" s="5" t="e">
-        <f>IF(A98="№ п/п",1,A98+1)</f>
+        <f t="shared" ref="A99:A124" si="6">IF(A98="№ п/п",1,A98+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B99" s="6" t="s">
@@ -6539,9 +6539,9 @@
         <v>8251006592</v>
       </c>
     </row>
-    <row r="100" ht="51" hidden="1" spans="1:15">
+    <row r="100" ht="51" spans="1:15">
       <c r="A100" s="5" t="e">
-        <f>IF(A99="№ п/п",1,A99+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B100" s="6" t="s">
@@ -6588,9 +6588,9 @@
         <v>8251006592</v>
       </c>
     </row>
-    <row r="101" ht="38.25" hidden="1" spans="1:15">
+    <row r="101" ht="38.25" spans="1:15">
       <c r="A101" s="5" t="e">
-        <f>IF(A100="№ п/п",1,A100+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B101" s="6" t="s">
@@ -6637,9 +6637,9 @@
         <v>8251006495</v>
       </c>
     </row>
-    <row r="102" ht="38.25" hidden="1" spans="1:15">
+    <row r="102" ht="38.25" spans="1:15">
       <c r="A102" s="5" t="e">
-        <f>IF(A101="№ п/п",1,A101+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B102" s="6" t="s">
@@ -6686,9 +6686,9 @@
         <v>8251006495</v>
       </c>
     </row>
-    <row r="103" ht="38.25" hidden="1" spans="1:15">
+    <row r="103" ht="38.25" spans="1:15">
       <c r="A103" s="5" t="e">
-        <f>IF(A102="№ п/п",1,A102+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B103" s="6" t="s">
@@ -6735,9 +6735,9 @@
         <v>8251006582</v>
       </c>
     </row>
-    <row r="104" ht="38.25" hidden="1" spans="1:15">
+    <row r="104" ht="38.25" spans="1:15">
       <c r="A104" s="5" t="e">
-        <f>IF(A103="№ п/п",1,A103+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B104" s="6" t="s">
@@ -6784,9 +6784,9 @@
         <v>8251006582</v>
       </c>
     </row>
-    <row r="105" ht="38.25" hidden="1" spans="1:15">
+    <row r="105" ht="38.25" spans="1:15">
       <c r="A105" s="5" t="e">
-        <f>IF(A104="№ п/п",1,A104+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B105" s="6" t="s">
@@ -6833,9 +6833,9 @@
         <v>8251006596</v>
       </c>
     </row>
-    <row r="106" ht="51" hidden="1" spans="1:15">
+    <row r="106" ht="51" spans="1:15">
       <c r="A106" s="5" t="e">
-        <f>IF(A105="№ п/п",1,A105+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -6882,9 +6882,9 @@
         <v>8251006616</v>
       </c>
     </row>
-    <row r="107" ht="38.25" hidden="1" spans="1:15">
+    <row r="107" ht="38.25" spans="1:15">
       <c r="A107" s="5" t="e">
-        <f>IF(A106="№ п/п",1,A106+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B107" s="6" t="s">
@@ -6924,16 +6924,16 @@
         <v>51</v>
       </c>
       <c r="N107" s="13" t="str">
-        <f t="shared" ref="N107:N124" si="5">"C1358318"</f>
+        <f t="shared" ref="N107:N125" si="7">"C1358318"</f>
         <v>C1358318</v>
       </c>
       <c r="O107" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="108" ht="38.25" hidden="1" spans="1:15">
+    <row r="108" ht="38.25" spans="1:15">
       <c r="A108" s="5" t="e">
-        <f>IF(A107="№ п/п",1,A107+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B108" s="6" t="s">
@@ -6973,16 +6973,16 @@
         <v>51</v>
       </c>
       <c r="N108" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O108" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="109" ht="38.25" hidden="1" spans="1:15">
+    <row r="109" ht="38.25" spans="1:15">
       <c r="A109" s="5" t="e">
-        <f>IF(A108="№ п/п",1,A108+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B109" s="6" t="s">
@@ -7022,16 +7022,16 @@
         <v>51</v>
       </c>
       <c r="N109" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O109" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="110" ht="38.25" hidden="1" spans="1:15">
+    <row r="110" ht="38.25" spans="1:15">
       <c r="A110" s="5" t="e">
-        <f>IF(A109="№ п/п",1,A109+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B110" s="6" t="s">
@@ -7071,16 +7071,16 @@
         <v>51</v>
       </c>
       <c r="N110" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O110" s="14">
         <v>8251006577</v>
       </c>
     </row>
-    <row r="111" ht="38.25" hidden="1" spans="1:15">
+    <row r="111" ht="38.25" spans="1:15">
       <c r="A111" s="5" t="e">
-        <f>IF(A110="№ п/п",1,A110+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B111" s="6" t="s">
@@ -7120,16 +7120,16 @@
         <v>51</v>
       </c>
       <c r="N111" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O111" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="112" ht="38.25" hidden="1" spans="1:15">
+    <row r="112" ht="38.25" spans="1:15">
       <c r="A112" s="5" t="e">
-        <f>IF(A111="№ п/п",1,A111+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B112" s="6" t="s">
@@ -7169,16 +7169,16 @@
         <v>51</v>
       </c>
       <c r="N112" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O112" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="113" ht="38.25" hidden="1" spans="1:15">
+    <row r="113" ht="38.25" spans="1:15">
       <c r="A113" s="5" t="e">
-        <f>IF(A112="№ п/п",1,A112+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B113" s="6" t="s">
@@ -7218,16 +7218,16 @@
         <v>51</v>
       </c>
       <c r="N113" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O113" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="114" ht="38.25" hidden="1" spans="1:15">
+    <row r="114" ht="38.25" spans="1:15">
       <c r="A114" s="5" t="e">
-        <f>IF(A113="№ п/п",1,A113+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B114" s="6" t="s">
@@ -7267,16 +7267,16 @@
         <v>51</v>
       </c>
       <c r="N114" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O114" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="115" ht="38.25" hidden="1" spans="1:15">
+    <row r="115" ht="38.25" spans="1:15">
       <c r="A115" s="5" t="e">
-        <f>IF(A114="№ п/п",1,A114+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B115" s="6" t="s">
@@ -7316,16 +7316,16 @@
         <v>51</v>
       </c>
       <c r="N115" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O115" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="116" ht="38.25" hidden="1" spans="1:15">
+    <row r="116" ht="38.25" spans="1:15">
       <c r="A116" s="5" t="e">
-        <f>IF(A115="№ п/п",1,A115+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B116" s="6" t="s">
@@ -7365,16 +7365,16 @@
         <v>51</v>
       </c>
       <c r="N116" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O116" s="14">
         <v>8251006577</v>
       </c>
     </row>
-    <row r="117" ht="38.25" hidden="1" spans="1:15">
+    <row r="117" ht="38.25" spans="1:15">
       <c r="A117" s="5" t="e">
-        <f>IF(A116="№ п/п",1,A116+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B117" s="6" t="s">
@@ -7414,16 +7414,16 @@
         <v>51</v>
       </c>
       <c r="N117" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O117" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="118" ht="38.25" hidden="1" spans="1:15">
+    <row r="118" ht="38.25" spans="1:15">
       <c r="A118" s="5" t="e">
-        <f>IF(A117="№ п/п",1,A117+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B118" s="6" t="s">
@@ -7463,16 +7463,16 @@
         <v>51</v>
       </c>
       <c r="N118" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O118" s="14">
         <v>8251006577</v>
       </c>
     </row>
-    <row r="119" ht="38.25" hidden="1" spans="1:15">
+    <row r="119" ht="38.25" spans="1:15">
       <c r="A119" s="5" t="e">
-        <f>IF(A118="№ п/п",1,A118+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B119" s="6" t="s">
@@ -7512,16 +7512,16 @@
         <v>51</v>
       </c>
       <c r="N119" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O119" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="120" ht="38.25" hidden="1" spans="1:15">
+    <row r="120" ht="38.25" spans="1:15">
       <c r="A120" s="5" t="e">
-        <f>IF(A119="№ п/п",1,A119+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B120" s="6" t="s">
@@ -7561,16 +7561,16 @@
         <v>51</v>
       </c>
       <c r="N120" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O120" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="121" ht="38.25" hidden="1" spans="1:15">
+    <row r="121" ht="38.25" spans="1:15">
       <c r="A121" s="5" t="e">
-        <f>IF(A120="№ п/п",1,A120+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B121" s="6" t="s">
@@ -7610,16 +7610,16 @@
         <v>51</v>
       </c>
       <c r="N121" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O121" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="122" ht="38.25" hidden="1" spans="1:15">
+    <row r="122" ht="38.25" spans="1:15">
       <c r="A122" s="5" t="e">
-        <f>IF(A121="№ п/п",1,A121+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B122" s="6" t="s">
@@ -7659,16 +7659,16 @@
         <v>51</v>
       </c>
       <c r="N122" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O122" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="123" ht="38.25" hidden="1" spans="1:15">
+    <row r="123" ht="38.25" spans="1:15">
       <c r="A123" s="5" t="e">
-        <f>IF(A122="№ п/п",1,A122+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B123" s="6" t="s">
@@ -7708,16 +7708,16 @@
         <v>51</v>
       </c>
       <c r="N123" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O123" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="124" ht="38.25" hidden="1" spans="1:15">
+    <row r="124" ht="38.25" spans="1:15">
       <c r="A124" s="5" t="e">
-        <f>IF(A123="№ п/п",1,A123+1)</f>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="B124" s="6" t="s">
@@ -7757,14 +7757,14 @@
         <v>51</v>
       </c>
       <c r="N124" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O124" s="14">
         <v>8251006657</v>
       </c>
     </row>
-    <row r="125" ht="38.25" hidden="1" spans="1:15">
+    <row r="125" ht="38.25" spans="1:15">
       <c r="A125" s="5" t="e">
         <f>IF(#REF!="№ п/п",1,#REF!+1)</f>
         <v>#REF!</v>
@@ -7806,7 +7806,7 @@
         <v>51</v>
       </c>
       <c r="N125" s="8" t="str">
-        <f>"C1358318"</f>
+        <f t="shared" si="7"/>
         <v>C1358318</v>
       </c>
       <c r="O125" s="12">
@@ -7839,7 +7839,7 @@
     </row>
     <row r="129" ht="15" spans="2:10">
       <c r="B129" s="16">
-        <f t="shared" ref="B129:B135" si="6">IF(B128="№ п/п",1,B128+1)</f>
+        <f t="shared" ref="B129:B135" si="8">IF(B128="№ п/п",1,B128+1)</f>
         <v>1</v>
       </c>
       <c r="C129" s="16" t="s">
@@ -7856,7 +7856,7 @@
     </row>
     <row r="130" ht="15" spans="2:10">
       <c r="B130" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="C130" s="16" t="s">
@@ -7875,7 +7875,7 @@
     </row>
     <row r="131" ht="15" spans="2:10">
       <c r="B131" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="C131" s="16" t="s">
@@ -7894,7 +7894,7 @@
     </row>
     <row r="132" ht="15" spans="2:10">
       <c r="B132" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="C132" s="16" t="s">
@@ -7911,7 +7911,7 @@
     </row>
     <row r="133" ht="15" spans="2:10">
       <c r="B133" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="C133" s="16" t="s">
@@ -7930,7 +7930,7 @@
     </row>
     <row r="134" ht="15" spans="2:10">
       <c r="B134" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="C134" s="16" t="s">
@@ -7949,7 +7949,7 @@
     </row>
     <row r="135" ht="15" spans="2:10">
       <c r="B135" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="C135" s="16" t="s">
@@ -8203,13 +8203,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:O125">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="814"/>
-        <filter val="835"/>
-        <filter val="666"/>
-      </filters>
-    </filterColumn>
     <extLst/>
   </autoFilter>
   <pageMargins left="0.354330708661417" right="0.15748031496063" top="0.984251968503937" bottom="0.984251968503937" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>